<commit_message>
remove the use of db
</commit_message>
<xml_diff>
--- a/app/views/templates/cheo/manager.xlsx
+++ b/app/views/templates/cheo/manager.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="考え方- Tu duy" sheetId="4" r:id="rId1"/>
-    <sheet name="熱意- Nhiet tinh" sheetId="5" r:id="rId2"/>
-    <sheet name="Vai trò -Manager" sheetId="6" r:id="rId3"/>
+    <sheet name="考え方- tu_duy" sheetId="4" r:id="rId1"/>
+    <sheet name="熱意- nhiet_tinh" sheetId="5" r:id="rId2"/>
+    <sheet name="manager- vai_tro" sheetId="6" r:id="rId3"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
@@ -39,74 +39,6 @@
   </si>
   <si>
     <t>レビュー
-Review- anh Lâm</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Tri</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Tài</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Thịnh</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Linh</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Lệ</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Long</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Nhu</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Đạt</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Dũng</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Nam</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Khương</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Thuận</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Thảo(nữ)</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Tuấn Anh</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Thảo (nam)</t>
-  </si>
-  <si>
-    <t>レビュー
-Review- Minh</t>
-  </si>
-  <si>
-    <t>レビュー
 Review</t>
   </si>
   <si>
@@ -1415,6 +1347,74 @@
   </si>
   <si>
     <t>役割評価</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- DangThanhLam</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenMinhTri</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- TranPhatTai</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- DangPhatThinh</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- LeThiThuyLinh</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenThiNhatLe</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- LeMinhLong</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- DangHoangNhu</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- TranTienDat</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- DinHienDung</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- MaiNhatNam</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenLeKhuong</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- TranKhanhThuan</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenHuynhThanhThao</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- PhamTuanAnh</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenVanThao</t>
+  </si>
+  <si>
+    <t>レビュー
+Review- NguyenQuangMinh</t>
   </si>
 </sst>
 </file>
@@ -1626,7 +1626,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1667,12 +1667,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6D9F0"/>
-        <bgColor rgb="FFC6D9F0"/>
       </patternFill>
     </fill>
   </fills>
@@ -1799,7 +1793,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
@@ -1905,9 +1899,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
@@ -2299,11 +2290,11 @@
   </sheetPr>
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R32" sqref="R32"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2333,67 +2324,67 @@
       </c>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:23" s="6" customFormat="1" ht="78.75">
+    <row r="2" spans="1:23" s="6" customFormat="1" ht="90">
       <c r="C2" s="7"/>
       <c r="D2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="U2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="V2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="W2" s="10" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="24">
@@ -2401,7 +2392,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D3" s="13"/>
       <c r="F3" s="14"/>
@@ -2436,7 +2427,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D4" s="13"/>
       <c r="F4" s="14"/>
@@ -2471,7 +2462,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D5" s="13"/>
       <c r="F5" s="14"/>
@@ -2503,13 +2494,13 @@
     </row>
     <row r="6" spans="1:23" ht="30">
       <c r="A6" s="17" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B6" s="11">
         <v>4</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D6" s="13"/>
       <c r="F6" s="14"/>
@@ -2541,13 +2532,13 @@
     </row>
     <row r="7" spans="1:23" ht="30">
       <c r="A7" s="17" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B7" s="11">
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D7" s="13"/>
       <c r="F7" s="14"/>
@@ -2582,7 +2573,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D8" s="13"/>
       <c r="F8" s="14"/>
@@ -2614,13 +2605,13 @@
     </row>
     <row r="9" spans="1:23" ht="30">
       <c r="A9" s="17" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B9" s="11">
         <v>7</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D9" s="13"/>
       <c r="F9" s="14"/>
@@ -2655,7 +2646,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D10" s="13"/>
       <c r="F10" s="14"/>
@@ -2690,7 +2681,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D11" s="13"/>
       <c r="F11" s="14"/>
@@ -2722,13 +2713,13 @@
     </row>
     <row r="12" spans="1:23" ht="24">
       <c r="A12" s="3" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B12" s="11">
         <v>10</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D12" s="13"/>
       <c r="F12" s="14"/>
@@ -2763,7 +2754,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D13" s="13"/>
       <c r="F13" s="14"/>
@@ -2798,7 +2789,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D14" s="13"/>
       <c r="F14" s="14"/>
@@ -2833,7 +2824,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="D15" s="13"/>
       <c r="F15" s="14"/>
@@ -2868,7 +2859,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D16" s="13"/>
       <c r="F16" s="14"/>
@@ -2900,13 +2891,13 @@
     </row>
     <row r="17" spans="1:23" ht="30">
       <c r="A17" s="17" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B17" s="11">
         <v>15</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D17" s="13"/>
       <c r="F17" s="14"/>
@@ -2941,7 +2932,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="D18" s="13"/>
       <c r="F18" s="14"/>
@@ -2976,7 +2967,7 @@
         <v>17</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D19" s="13"/>
       <c r="F19" s="14"/>
@@ -3011,7 +3002,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D20" s="13"/>
       <c r="F20" s="14"/>
@@ -3043,13 +3034,13 @@
     </row>
     <row r="21" spans="1:23" ht="30">
       <c r="A21" s="17" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B21" s="11">
         <v>19</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D21" s="13"/>
       <c r="F21" s="14"/>
@@ -3084,7 +3075,7 @@
         <v>20</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D22" s="13"/>
       <c r="F22" s="14"/>
@@ -3119,7 +3110,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D23" s="13"/>
       <c r="F23" s="18"/>
@@ -3154,7 +3145,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D24" s="13"/>
       <c r="U24" s="15" t="e">
@@ -3174,7 +3165,7 @@
         <v>23</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="D25" s="13"/>
       <c r="U25" s="15" t="e">
@@ -3194,7 +3185,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="D26" s="13"/>
       <c r="U26" s="15" t="e">
@@ -3214,7 +3205,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D27" s="13"/>
       <c r="U27" s="15" t="e">
@@ -3230,10 +3221,10 @@
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="B28" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="38"/>
+      <c r="B28" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="37"/>
       <c r="D28" s="3">
         <f>SUM(D3:D27)</f>
         <v>0</v>
@@ -3309,10 +3300,10 @@
     </row>
     <row r="30" spans="1:23" ht="36">
       <c r="B30" s="20" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D30" s="22"/>
     </row>
@@ -3321,7 +3312,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D31" s="24"/>
     </row>
@@ -3330,7 +3321,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D32" s="24"/>
     </row>
@@ -3339,7 +3330,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="D33" s="24"/>
     </row>
@@ -3348,7 +3339,7 @@
         <v>0</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="D34" s="24"/>
     </row>
@@ -3357,7 +3348,7 @@
         <v>-2</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D35" s="24"/>
     </row>
@@ -3366,7 +3357,7 @@
         <v>-5</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D36" s="24"/>
     </row>
@@ -3375,7 +3366,7 @@
         <v>-10</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D37" s="24"/>
     </row>
@@ -3399,7 +3390,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F28" sqref="F28:U28"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3421,10 +3412,10 @@
   <sheetData>
     <row r="1" spans="1:24" ht="33.75">
       <c r="A1" s="1" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
@@ -3432,67 +3423,67 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
     </row>
-    <row r="2" spans="1:24" s="6" customFormat="1" ht="78.75">
+    <row r="2" spans="1:24" s="6" customFormat="1" ht="90">
       <c r="C2" s="7"/>
       <c r="E2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="V2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="W2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="X2" s="10" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="24">
@@ -3500,12 +3491,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="40"/>
+        <v>76</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="39"/>
       <c r="E3" s="13"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -3539,12 +3530,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="40"/>
+        <v>76</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="39"/>
       <c r="E4" s="13"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3578,12 +3569,12 @@
         <v>3</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="40"/>
+        <v>76</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="39"/>
       <c r="E5" s="13"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3617,12 +3608,12 @@
         <v>4</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="42"/>
+        <v>76</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="41"/>
       <c r="E6" s="13"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3656,12 +3647,12 @@
         <v>5</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>92</v>
-      </c>
-      <c r="D7" s="40"/>
+        <v>76</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="39"/>
       <c r="E7" s="13"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3695,12 +3686,12 @@
         <v>6</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="D8" s="40"/>
+        <v>70</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="39"/>
       <c r="E8" s="13"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -3734,12 +3725,12 @@
         <v>7</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C9" s="41" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="42"/>
+        <v>70</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="41"/>
       <c r="E9" s="13"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -3773,12 +3764,12 @@
         <v>8</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="40"/>
+        <v>70</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="39"/>
       <c r="E10" s="13"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -3812,12 +3803,12 @@
         <v>9</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C11" s="39" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="40"/>
+        <v>70</v>
+      </c>
+      <c r="C11" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="39"/>
       <c r="E11" s="13"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -3851,12 +3842,12 @@
         <v>10</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D12" s="40"/>
+        <v>70</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="39"/>
       <c r="E12" s="13"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -3890,12 +3881,12 @@
         <v>11</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="D13" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="39"/>
       <c r="E13" s="13"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -3929,12 +3920,12 @@
         <v>12</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="39"/>
       <c r="E14" s="13"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -3968,12 +3959,12 @@
         <v>13</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="39"/>
       <c r="E15" s="13"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -4007,12 +3998,12 @@
         <v>14</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="39"/>
       <c r="E16" s="13"/>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -4046,12 +4037,12 @@
         <v>15</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="39"/>
       <c r="E17" s="13"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -4085,12 +4076,12 @@
         <v>16</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="40"/>
+        <v>63</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="39"/>
       <c r="E18" s="13"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -4124,12 +4115,12 @@
         <v>17</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="40"/>
+        <v>60</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="39"/>
       <c r="E19" s="13"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -4163,12 +4154,12 @@
         <v>18</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="40"/>
+        <v>60</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="39"/>
       <c r="E20" s="13"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -4202,12 +4193,12 @@
         <v>19</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="40"/>
+        <v>52</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="39"/>
       <c r="E21" s="13"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -4241,12 +4232,12 @@
         <v>20</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="40"/>
+        <v>52</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" s="39"/>
       <c r="E22" s="13"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -4280,12 +4271,12 @@
         <v>21</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="40"/>
+        <v>52</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="39"/>
       <c r="E23" s="13"/>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
@@ -4319,12 +4310,12 @@
         <v>22</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="42"/>
+        <v>52</v>
+      </c>
+      <c r="C24" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" s="41"/>
       <c r="E24" s="13"/>
       <c r="V24" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4343,12 +4334,12 @@
         <v>23</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="42"/>
+        <v>52</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="41"/>
       <c r="E25" s="13"/>
       <c r="V25" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4367,12 +4358,12 @@
         <v>24</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="40"/>
+        <v>52</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="39"/>
       <c r="E26" s="13"/>
       <c r="V26" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4391,12 +4382,12 @@
         <v>25</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D27" s="42"/>
+        <v>52</v>
+      </c>
+      <c r="C27" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="41"/>
       <c r="E27" s="13"/>
       <c r="V27" s="15" t="e">
         <f t="shared" si="0"/>
@@ -4411,11 +4402,11 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="B28" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
+      <c r="B28" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
       <c r="E28" s="3">
         <f t="shared" ref="E28:U28" si="2">SUM(E3:E27)</f>
         <v>0</v>
@@ -4492,72 +4483,72 @@
     </row>
     <row r="30" spans="1:24" ht="24">
       <c r="B30" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C30" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="44"/>
+        <v>35</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="43"/>
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:24" ht="51.75" customHeight="1">
       <c r="B31" s="11">
         <v>5</v>
       </c>
-      <c r="C31" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="45"/>
+      <c r="C31" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="44"/>
       <c r="E31" s="24"/>
     </row>
     <row r="32" spans="1:24" ht="33.75" customHeight="1">
       <c r="B32" s="11">
         <v>4</v>
       </c>
-      <c r="C32" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="43"/>
+      <c r="C32" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="42"/>
       <c r="E32" s="24"/>
     </row>
     <row r="33" spans="2:5" ht="30" customHeight="1">
       <c r="B33" s="11">
         <v>3</v>
       </c>
-      <c r="C33" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="D33" s="43"/>
+      <c r="C33" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="42"/>
       <c r="E33" s="24"/>
     </row>
     <row r="34" spans="2:5" ht="31.5" customHeight="1">
       <c r="B34" s="11">
         <v>2</v>
       </c>
-      <c r="C34" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="43"/>
+      <c r="C34" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="42"/>
       <c r="E34" s="24"/>
     </row>
     <row r="35" spans="2:5" ht="39" customHeight="1">
       <c r="B35" s="11">
         <v>1</v>
       </c>
-      <c r="C35" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D35" s="43"/>
+      <c r="C35" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="42"/>
       <c r="E35" s="24"/>
     </row>
     <row r="36" spans="2:5" ht="36.75" customHeight="1">
       <c r="B36" s="11">
         <v>0</v>
       </c>
-      <c r="C36" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="43"/>
+      <c r="C36" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="42"/>
       <c r="E36" s="24"/>
     </row>
   </sheetData>
@@ -4573,18 +4564,18 @@
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C17:D17"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C11:D11"/>
@@ -4608,11 +4599,11 @@
   </sheetPr>
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE20" sqref="AE20"/>
+      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4629,89 +4620,89 @@
   <sheetData>
     <row r="1" spans="1:24" ht="33.75">
       <c r="A1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>131</v>
+        <v>115</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>114</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="47.25">
+    <row r="2" spans="1:24" ht="90">
       <c r="E2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="W2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="X2" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A3" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C3" s="34">
         <v>1</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="16"/>
@@ -4729,16 +4720,16 @@
     </row>
     <row r="4" spans="1:24" s="14" customFormat="1" ht="29.1" customHeight="1">
       <c r="A4" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C4" s="34">
         <v>2</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="E4" s="32"/>
       <c r="F4" s="16"/>
@@ -4756,16 +4747,16 @@
     </row>
     <row r="5" spans="1:24" s="14" customFormat="1" ht="29.1" customHeight="1">
       <c r="A5" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C5" s="34">
         <v>3</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="16"/>
@@ -4783,16 +4774,16 @@
     </row>
     <row r="6" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A6" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C6" s="34">
         <v>4</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E6" s="32"/>
       <c r="F6" s="16"/>
@@ -4810,16 +4801,16 @@
     </row>
     <row r="7" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A7" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C7" s="34">
         <v>5</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E7" s="32"/>
       <c r="F7" s="16"/>
@@ -4837,16 +4828,16 @@
     </row>
     <row r="8" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A8" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C8" s="34">
         <v>6</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="E8" s="32"/>
       <c r="F8" s="16"/>
@@ -4864,16 +4855,16 @@
     </row>
     <row r="9" spans="1:24" s="14" customFormat="1" ht="33.6" customHeight="1">
       <c r="A9" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C9" s="34">
         <v>7</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="16"/>
@@ -4891,16 +4882,16 @@
     </row>
     <row r="10" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A10" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C10" s="34">
         <v>8</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="E10" s="32"/>
       <c r="F10" s="16"/>
@@ -4918,16 +4909,16 @@
     </row>
     <row r="11" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A11" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C11" s="34">
         <v>9</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="E11" s="32"/>
       <c r="F11" s="16"/>
@@ -4945,16 +4936,16 @@
     </row>
     <row r="12" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A12" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C12" s="34">
         <v>10</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="E12" s="32"/>
       <c r="F12" s="16"/>
@@ -4972,16 +4963,16 @@
     </row>
     <row r="13" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A13" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C13" s="34">
         <v>11</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="E13" s="32"/>
       <c r="F13" s="16"/>
@@ -4999,16 +4990,16 @@
     </row>
     <row r="14" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A14" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C14" s="34">
         <v>12</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="16"/>
@@ -5026,16 +5017,16 @@
     </row>
     <row r="15" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A15" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C15" s="34">
         <v>13</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="16"/>
@@ -5053,16 +5044,16 @@
     </row>
     <row r="16" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A16" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C16" s="34">
         <v>14</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="E16" s="32"/>
       <c r="F16" s="16"/>
@@ -5080,16 +5071,16 @@
     </row>
     <row r="17" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A17" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C17" s="34">
         <v>15</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="E17" s="32"/>
       <c r="F17" s="16"/>
@@ -5107,16 +5098,16 @@
     </row>
     <row r="18" spans="1:24" s="14" customFormat="1" ht="15.75">
       <c r="A18" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C18" s="34">
         <v>16</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="16"/>
@@ -5134,16 +5125,16 @@
     </row>
     <row r="19" spans="1:24" s="14" customFormat="1" ht="47.1" customHeight="1">
       <c r="A19" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C19" s="34">
         <v>17</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E19" s="32"/>
       <c r="F19" s="16"/>
@@ -5161,16 +5152,16 @@
     </row>
     <row r="20" spans="1:24" s="14" customFormat="1" ht="15.75">
       <c r="A20" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C20" s="34">
         <v>18</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="E20" s="32"/>
       <c r="F20" s="16"/>
@@ -5188,16 +5179,16 @@
     </row>
     <row r="21" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A21" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C21" s="34">
         <v>19</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="E21" s="32"/>
       <c r="F21" s="16"/>
@@ -5215,16 +5206,16 @@
     </row>
     <row r="22" spans="1:24" s="14" customFormat="1" ht="31.5">
       <c r="A22" s="35" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="C22" s="34">
         <v>20</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="16"/>
@@ -5241,11 +5232,11 @@
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75">
-      <c r="B23" s="48" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="50"/>
+      <c r="B23" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="18">
         <f t="shared" ref="E23:U23" si="2">SUM(E3:E22)</f>
         <v>0</v>
@@ -5327,66 +5318,66 @@
     </row>
     <row r="26" spans="1:24" ht="60">
       <c r="B26" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="51"/>
+        <v>90</v>
+      </c>
+      <c r="C26" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="50"/>
     </row>
     <row r="27" spans="1:24" ht="31.5" customHeight="1">
       <c r="B27" s="30">
         <v>5</v>
       </c>
-      <c r="C27" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27" s="47"/>
+      <c r="C27" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="46"/>
     </row>
     <row r="28" spans="1:24" ht="31.5" customHeight="1">
       <c r="B28" s="30">
         <v>4</v>
       </c>
-      <c r="C28" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="47"/>
+      <c r="C28" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="46"/>
     </row>
     <row r="29" spans="1:24" ht="31.5" customHeight="1">
       <c r="B29" s="30">
         <v>3</v>
       </c>
-      <c r="C29" s="46" t="s">
-        <v>103</v>
-      </c>
-      <c r="D29" s="47"/>
+      <c r="C29" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="D29" s="46"/>
     </row>
     <row r="30" spans="1:24" ht="31.5" customHeight="1">
       <c r="B30" s="30">
         <v>2</v>
       </c>
-      <c r="C30" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="47"/>
+      <c r="C30" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="46"/>
     </row>
     <row r="31" spans="1:24" ht="31.5" customHeight="1">
       <c r="B31" s="30">
         <v>1</v>
       </c>
-      <c r="C31" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="D31" s="47"/>
+      <c r="C31" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" s="46"/>
     </row>
     <row r="32" spans="1:24" ht="31.5" customHeight="1">
       <c r="B32" s="30">
         <v>0</v>
       </c>
-      <c r="C32" s="46" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" s="47"/>
+      <c r="C32" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>